<commit_message>
Added Paul's section. Fixed the bib file for conflicts. Compiles fine.
</commit_message>
<xml_diff>
--- a/Abbreviations.xlsx
+++ b/Abbreviations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhernand\Desktop\Review-Paper-Progress-in-Biomedical-Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B87EF9-2CC6-4FD2-85E0-D4C5E5DA66CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D981CC-FAC4-47A9-B612-F6F8D169464E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{4234119A-B9FA-404B-BB17-584A2842C4F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Mathematical terms</t>
   </si>
@@ -36,39 +36,21 @@
     <t>ODE</t>
   </si>
   <si>
-    <t>(RD-)PDE</t>
-  </si>
-  <si>
-    <t>DDE</t>
-  </si>
-  <si>
     <t>1/2/3D</t>
   </si>
   <si>
     <t>AMD</t>
   </si>
   <si>
-    <t>nAMD</t>
-  </si>
-  <si>
     <t>nnAMD</t>
   </si>
   <si>
-    <t>CNV</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
     <t>BrM</t>
   </si>
   <si>
     <t>CC</t>
   </si>
   <si>
-    <t>Ngb</t>
-  </si>
-  <si>
     <t>ILM</t>
   </si>
   <si>
@@ -78,12 +60,6 @@
     <t>OS</t>
   </si>
   <si>
-    <t>Ph</t>
-  </si>
-  <si>
-    <t>Ch</t>
-  </si>
-  <si>
     <t>RPE</t>
   </si>
   <si>
@@ -93,12 +69,6 @@
     <t>RP</t>
   </si>
   <si>
-    <t>RCD</t>
-  </si>
-  <si>
-    <t>CORD</t>
-  </si>
-  <si>
     <t>Bruch’s membrane</t>
   </si>
   <si>
@@ -108,9 +78,6 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>FEM</t>
-  </si>
-  <si>
     <t>Age-related macular degeneration</t>
   </si>
   <si>
@@ -126,48 +93,21 @@
     <t>PO$_2$</t>
   </si>
   <si>
-    <t>BC</t>
-  </si>
-  <si>
-    <t>Boundary condition</t>
-  </si>
-  <si>
     <t>Inner limiting membrane</t>
   </si>
   <si>
-    <t>Outer plexiform layer</t>
-  </si>
-  <si>
-    <t>OPL</t>
-  </si>
-  <si>
     <t>Retinal pigment epithelium</t>
   </si>
   <si>
     <t>Inner segment(s)</t>
   </si>
   <si>
-    <t>Dark adaptation</t>
-  </si>
-  <si>
-    <t>DA</t>
-  </si>
-  <si>
     <t>LA</t>
   </si>
   <si>
     <t>Light adaptation</t>
   </si>
   <si>
-    <t>IPL</t>
-  </si>
-  <si>
-    <t>Inner plexiform layer</t>
-  </si>
-  <si>
-    <t>Neuroglobin</t>
-  </si>
-  <si>
     <t>Ordinary differential equation</t>
   </si>
   <si>
@@ -177,156 +117,30 @@
     <t>DRC</t>
   </si>
   <si>
-    <t>(SD-)OCT</t>
-  </si>
-  <si>
-    <t>(Spectral-domain) optical coherence tomography</t>
-  </si>
-  <si>
-    <t>OCTA</t>
-  </si>
-  <si>
-    <t>Optical coherence tomography angiography</t>
-  </si>
-  <si>
-    <t>Rod-cone dystrophy</t>
-  </si>
-  <si>
-    <t>Cone-rod dystrophy</t>
-  </si>
-  <si>
-    <t>RdCVF(1/2)(L)</t>
-  </si>
-  <si>
-    <t>Rod-derived cone viability factor(1/2)(-long)</t>
-  </si>
-  <si>
     <t>BSG1</t>
   </si>
   <si>
     <t>Basigin-1</t>
   </si>
   <si>
-    <t>GLUT1</t>
-  </si>
-  <si>
-    <t>Glucose transporter 1</t>
-  </si>
-  <si>
-    <t>FAF</t>
-  </si>
-  <si>
-    <t>Fundus autofluorescence</t>
-  </si>
-  <si>
-    <t>CFP</t>
-  </si>
-  <si>
-    <t>Colour fundus photography</t>
-  </si>
-  <si>
-    <t>Infrared reflectance</t>
-  </si>
-  <si>
-    <t>IR</t>
-  </si>
-  <si>
-    <t>AOSLO</t>
-  </si>
-  <si>
-    <t>Adaptive optics scanning laser ophthalmoscopy</t>
-  </si>
-  <si>
-    <t>(P/mf)ERG</t>
-  </si>
-  <si>
-    <t>(Pattern/multi-focal) electroretinogram</t>
-  </si>
-  <si>
-    <t>Docosahexaenoic acid</t>
-  </si>
-  <si>
-    <t>DHA</t>
-  </si>
-  <si>
     <t>Outer segment(s)</t>
   </si>
   <si>
-    <t>Photoreceptor(s)</t>
-  </si>
-  <si>
-    <t>Delay differential equation</t>
-  </si>
-  <si>
     <t>(Reaction-diffusion) partial differential equation</t>
   </si>
   <si>
     <t>1/2/3 spatial dimensions</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>G6P</t>
-  </si>
-  <si>
-    <t>F16BP</t>
-  </si>
-  <si>
-    <t>G3P</t>
-  </si>
-  <si>
-    <t>NADPH</t>
-  </si>
-  <si>
-    <t>PYR</t>
-  </si>
-  <si>
     <t>LACT</t>
   </si>
   <si>
     <t>Reactive oxygen species</t>
   </si>
   <si>
-    <t>ACoA</t>
-  </si>
-  <si>
-    <t>CIT</t>
-  </si>
-  <si>
-    <t>PACF</t>
-  </si>
-  <si>
-    <t>Photoreceptor apoptosis commitment factor</t>
-  </si>
-  <si>
-    <t>Citrate</t>
-  </si>
-  <si>
-    <t>Acetyl coenzyme A</t>
-  </si>
-  <si>
     <t>Lactate</t>
   </si>
   <si>
-    <t>Pyruvate</t>
-  </si>
-  <si>
-    <t>Nicotinamide adenine dinucleotide phosphate</t>
-  </si>
-  <si>
-    <t>Glycerol-3-phosphate</t>
-  </si>
-  <si>
-    <t>Fructose-1,6-bisphosphate</t>
-  </si>
-  <si>
-    <t>Glucose-6-phosphate</t>
-  </si>
-  <si>
-    <t>Glucose</t>
-  </si>
-  <si>
     <t>MANF</t>
   </si>
   <si>
@@ -336,37 +150,10 @@
     <t>Non-neovascular AMD</t>
   </si>
   <si>
-    <t>Neovascular AMD</t>
-  </si>
-  <si>
-    <t>Choroidal neovascularisation</t>
-  </si>
-  <si>
-    <t>Geographic atrophy</t>
-  </si>
-  <si>
-    <t>Cholesterol</t>
-  </si>
-  <si>
-    <t>Finite element method</t>
-  </si>
-  <si>
     <t>ONL</t>
   </si>
   <si>
     <t>Outer nuclear layer</t>
-  </si>
-  <si>
-    <t>IRD</t>
-  </si>
-  <si>
-    <t>Inherited retinal disease</t>
-  </si>
-  <si>
-    <t>mTOR(C1)</t>
-  </si>
-  <si>
-    <t>Mammalian target of rapamycin (complex 1)</t>
   </si>
   <si>
     <t>IVI</t>
@@ -466,6 +253,15 @@
   </si>
   <si>
     <t>Validation, verification and uncertainty quantification</t>
+  </si>
+  <si>
+    <t>PDE</t>
+  </si>
+  <si>
+    <t>OCT</t>
+  </si>
+  <si>
+    <t>Optical coherence tomography</t>
   </si>
 </sst>
 </file>
@@ -549,18 +345,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,29 +668,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17560958-82B1-4A0A-83F0-B580EE94E5EA}">
-  <dimension ref="B2:C75"/>
+  <dimension ref="B2:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
@@ -908,200 +702,200 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>138</v>
+        <v>64</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>136</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>141</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>129</v>
+        <v>5</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>130</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
@@ -1109,368 +903,96 @@
         <v>73</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>133</v>
+        <v>41</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B73" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B75" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="B17:C72">
-    <sortCondition ref="B16:B72"/>
+  <sortState ref="B15:C38">
+    <sortCondition ref="B14:B38"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>